<commit_message>
Tabela da questao 3
</commit_message>
<xml_diff>
--- a/fogos3/valores.xlsx
+++ b/fogos3/valores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\IncendioFlorestal\fogos3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0843811-42EF-4363-8ADF-FE305B4EF896}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A74632-2EE4-443D-9189-7FE8D45F2274}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7920" xr2:uid="{5EDFCEA3-8978-4CAC-9DA6-606ADB9E568F}"/>
   </bookViews>
@@ -368,7 +368,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-03DC-4C8D-A223-31ED1EF1CC93}"/>
+              <c16:uniqueId val="{00000000-DA9E-4630-86C0-38A2C78EFB73}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -381,11 +381,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="2036560496"/>
-        <c:axId val="2081077344"/>
+        <c:axId val="44186736"/>
+        <c:axId val="2082533504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2036560496"/>
+        <c:axId val="44186736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -428,7 +428,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2081077344"/>
+        <c:crossAx val="2082533504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -436,7 +436,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2081077344"/>
+        <c:axId val="2082533504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -487,7 +487,7 @@
             <a:endParaRPr lang="pt-PT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2036560496"/>
+        <c:crossAx val="44186736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1109,10 +1109,10 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{736D281B-C200-40B2-B827-7272711337CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{004B15DC-2928-4942-A76B-D37E0A95763C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1433,7 +1433,7 @@
   <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection sqref="A1:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>